<commit_message>
QA overhaul: fix HTML template, diversify scripts, improve content quality across all 25 models
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/antonella/Antonella_Complete_Infloww.xlsx
+++ b/antonella/Antonella_Complete_Infloww.xlsx
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>can't stop thinking about earlier. you around? 💜</t>
+          <t>I made something special and you're the only one I want to show it to 💜</t>
         </is>
       </c>
       <c r="C2" s="5" t="inlineStr">
@@ -2350,7 +2350,7 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>hey hope you're good cutie, text me when you're back 🖤</t>
+          <t>miss talking to you cutie, where'd you go? 🖤</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>okay I guess you're busy. I might delete this later, it was only for you 💜</t>
+          <t>fine I'll just keep this to myself then 😏</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>you really need to see what I just did for you... trust me 🖤</t>
+          <t>I have something to show you but you're leaving me on read... 🖤</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>heyy? 🥺</t>
+          <t>helloooo 🥺</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
@@ -4217,7 +4217,7 @@
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>more...</t>
+          <t>again...</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>you have no idea what you're doing to me omg</t>
+          <t>I literally can't handle this right now</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>don't stop</t>
+          <t>keep going</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">

</xml_diff>

<commit_message>
QA Round 2: deep quality optimization - compliance, diversification, UX improvements
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/antonella/Antonella_Complete_Infloww.xlsx
+++ b/antonella/Antonella_Complete_Infloww.xlsx
@@ -38,9 +38,10 @@
     <sheet name="customno2" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="done1" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="done2" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="cumcontrol" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="dickpic" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="boosters" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="cumcontrol1" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="cumcontrol2" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="dickpic" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="boosters" sheetId="35" state="visible" r:id="rId35"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -642,7 +643,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>cum with me 🖤</t>
+          <t>I want us to finish together 🖤</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -659,7 +660,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>hold on</t>
+          <t>wait</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -702,7 +703,7 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>FUCK 🖤</t>
+          <t>fuckkkk 🖤</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
@@ -736,7 +737,7 @@
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>give me a sec</t>
+          <t>one second</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
@@ -753,7 +754,7 @@
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>I can't hold back anymore</t>
+          <t>I can't resist you anymore</t>
         </is>
       </c>
       <c r="C11" s="6" t="inlineStr"/>
@@ -894,7 +895,7 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>did you watch it? 🥺</t>
+          <t>did you see it? 🥺</t>
         </is>
       </c>
       <c r="C20" s="5" t="inlineStr">
@@ -928,7 +929,7 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>give me a sec 🖤</t>
+          <t>one second 🖤</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
@@ -3889,7 +3890,7 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>don't you dare finish before you see this, trust me you want to wait 🥺</t>
+          <t>if you finish before you see what I'm sending next you'll regret it 💜</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
@@ -3907,12 +3908,12 @@
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>hold it... wait until you see what I'm about to send, trust me it's worth it 🖤</t>
+          <t>wait wait wait... I have one more thing for you before you finish</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
         <is>
-          <t>DELAY.</t>
+          <t>DELAY. Send final PPV.</t>
         </is>
       </c>
       <c r="D3" s="13" t="inlineStr"/>
@@ -3925,12 +3926,12 @@
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>wait for me, I want us to finish together... open this first 💜</t>
+          <t>I want to feel it at the same time... watch this first</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
         <is>
-          <t>SYNC variant.</t>
+          <t>SYNC variant. Send PPV.</t>
         </is>
       </c>
       <c r="D4" s="13" t="inlineStr"/>
@@ -3943,12 +3944,12 @@
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>I'm so close too, cum with me... but you need to see this first 🖤</t>
+          <t>okay NOW we can go together... open this 🖤</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
         <is>
-          <t>SYNC. Final PPV.</t>
+          <t>SYNC. Send PPV.</t>
         </is>
       </c>
       <c r="D5" s="13" t="inlineStr"/>
@@ -3961,7 +3962,7 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>hold it, not yet... I need you to last a little longer for me pleaseee 💜</t>
+          <t>you better not be close already cutie... I have more to show you 💜</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
@@ -3979,12 +3980,12 @@
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>don't cum yet... I'm not done with you 🖤</t>
+          <t>not yet... I said not yet 🖤</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">
         <is>
-          <t>EDGE. More PPVs left.</t>
+          <t>CONTROL. More PPVs to send. Create urgency to open next.</t>
         </is>
       </c>
       <c r="D7" s="13" t="inlineStr"/>
@@ -4039,17 +4040,17 @@
     <row r="2">
       <c r="A2" s="13" t="inlineStr">
         <is>
-          <t>dpppv2</t>
+          <t>delay2</t>
         </is>
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>okay you just made me do something... give me a sec 🖤</t>
+          <t>hold on just a little longer, I promise this next one is worth it</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
         <is>
-          <t>LEVERAGE variant.</t>
+          <t>DELAY variant.</t>
         </is>
       </c>
       <c r="D2" s="13" t="inlineStr"/>
@@ -4057,17 +4058,17 @@
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
         <is>
-          <t>dpppv1</t>
+          <t>delay1</t>
         </is>
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>you can't just send me that and expect me not to do something about it, hold on 💜</t>
+          <t>don't you dare... not until you see what I just did 🖤</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
         <is>
-          <t>LEVERAGE. WAIT 1-2 min then send PPV.</t>
+          <t>DELAY. Send PPV.</t>
         </is>
       </c>
       <c r="D3" s="13" t="inlineStr"/>
@@ -4075,17 +4076,17 @@
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
         <is>
-          <t>dprapport2</t>
+          <t>sync2</t>
         </is>
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>omg I was not expecting that but... damn 🖤</t>
+          <t>let's do this together... but you have to open this first</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
         <is>
-          <t>DURING RAPPORT variant.</t>
+          <t>SYNC variant.</t>
         </is>
       </c>
       <c r="D4" s="13" t="inlineStr"/>
@@ -4093,17 +4094,17 @@
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
         <is>
-          <t>dprapport1</t>
+          <t>sync1</t>
         </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>woah you don't waste time huh? that's actually really hot though ngl 🥺</t>
+          <t>okay I'm ready now too... watch this with me 💜</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
         <is>
-          <t>DURING RAPPORT. She's 'shy' but reacts positively.</t>
+          <t>SYNC. Send PPV.</t>
         </is>
       </c>
       <c r="D5" s="13" t="inlineStr"/>
@@ -4111,17 +4112,17 @@
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
         <is>
-          <t>dpsext2</t>
+          <t>edge2</t>
         </is>
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>oh my god... that is... damn. I need to show you something right now 💜</t>
+          <t>patience... the best part hasn't even happened yet</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
         <is>
-          <t>DURING SEXTING variant.</t>
+          <t>EDGE variant.</t>
         </is>
       </c>
       <c r="D6" s="13" t="inlineStr"/>
@@ -4129,17 +4130,17 @@
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
         <is>
-          <t>dpsext1</t>
+          <t>edge1</t>
         </is>
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>fuck okay that's... wow. you have no idea what that just did to me 🖤</t>
+          <t>slow down cutie... I'm not letting you off that easy 🖤</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">
         <is>
-          <t>DURING SEXTING. React positively, leverage into PPV.</t>
+          <t>CONTROL.</t>
         </is>
       </c>
       <c r="D7" s="13" t="inlineStr"/>
@@ -4150,6 +4151,161 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="80" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>Text</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>*Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="13" t="inlineStr">
+        <is>
+          <t>dpppv2</t>
+        </is>
+      </c>
+      <c r="B2" s="13" t="inlineStr">
+        <is>
+          <t>okay you just made me do something... give me a sec 🖤</t>
+        </is>
+      </c>
+      <c r="C2" s="13" t="inlineStr">
+        <is>
+          <t>LEVERAGE variant.</t>
+        </is>
+      </c>
+      <c r="D2" s="13" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="13" t="inlineStr">
+        <is>
+          <t>dpppv1</t>
+        </is>
+      </c>
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t>you can't just send me that and expect me not to do something about it, hold on 💜</t>
+        </is>
+      </c>
+      <c r="C3" s="13" t="inlineStr">
+        <is>
+          <t>LEVERAGE. WAIT 1-2 min then send PPV.</t>
+        </is>
+      </c>
+      <c r="D3" s="13" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="13" t="inlineStr">
+        <is>
+          <t>dprapport2</t>
+        </is>
+      </c>
+      <c r="B4" s="13" t="inlineStr">
+        <is>
+          <t>omg I was not expecting that but... damn 🖤</t>
+        </is>
+      </c>
+      <c r="C4" s="13" t="inlineStr">
+        <is>
+          <t>DURING RAPPORT variant.</t>
+        </is>
+      </c>
+      <c r="D4" s="13" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="13" t="inlineStr">
+        <is>
+          <t>dprapport1</t>
+        </is>
+      </c>
+      <c r="B5" s="13" t="inlineStr">
+        <is>
+          <t>woah you don't waste time huh? that's actually really hot though ngl 🥺</t>
+        </is>
+      </c>
+      <c r="C5" s="13" t="inlineStr">
+        <is>
+          <t>DURING RAPPORT. She's 'shy' but reacts positively.</t>
+        </is>
+      </c>
+      <c r="D5" s="13" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="13" t="inlineStr">
+        <is>
+          <t>dpsext2</t>
+        </is>
+      </c>
+      <c r="B6" s="13" t="inlineStr">
+        <is>
+          <t>oh my god... that is... damn. I need to show you something right now 💜</t>
+        </is>
+      </c>
+      <c r="C6" s="13" t="inlineStr">
+        <is>
+          <t>DURING SEXTING variant.</t>
+        </is>
+      </c>
+      <c r="D6" s="13" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="13" t="inlineStr">
+        <is>
+          <t>dpsext1</t>
+        </is>
+      </c>
+      <c r="B7" s="13" t="inlineStr">
+        <is>
+          <t>fuck okay that's... wow. you have no idea what that just did to me 🖤</t>
+        </is>
+      </c>
+      <c r="C7" s="13" t="inlineStr">
+        <is>
+          <t>DURING SEXTING. React positively, leverage into PPV.</t>
+        </is>
+      </c>
+      <c r="D7" s="13" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
fix: sexting intensity escalation + PPV0 phase detection bug across all 23 models
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/antonella/Antonella_Complete_Infloww.xlsx
+++ b/antonella/Antonella_Complete_Infloww.xlsx
@@ -643,7 +643,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>I want us to finish together 🖤</t>
+          <t>let go with me babe... I need you to see this 💜</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -677,7 +677,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>I wanna finish with you... I'm so close omg</t>
+          <t>I'm cumming... right now... don't look away</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr"/>
@@ -690,7 +690,7 @@
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>don't cum yet pleaseee</t>
+          <t>I'm right there babe... don't go anywhere, I need you to watch me finish 💜</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr"/>
@@ -703,7 +703,7 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>fuckkkk 🖤</t>
+          <t>oh my god I can't take it 🖤</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
@@ -720,7 +720,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>this is the furthest I've ever gone for someone online... watch 💜</t>
+          <t>you need to see this... I've never been like this before 💜</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>I can't resist you anymore</t>
+          <t>I'm about to lose it... you need to see what's happening to me right now</t>
         </is>
       </c>
       <c r="C11" s="6" t="inlineStr"/>
@@ -767,7 +767,7 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>I keep thinking about you watching me while I touch myself and it's making everything worse 💜</t>
+          <t>I keep pushing my fingers deeper and moaning into my pillow... god this feels so good 💜</t>
         </is>
       </c>
       <c r="C12" s="5" t="inlineStr">
@@ -784,7 +784,7 @@
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>I need to cum so bad right now you have no idea</t>
+          <t>I'm rubbing my clit so hard right now and I can't slow down... my legs are shaking</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr"/>
@@ -797,7 +797,7 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>omg 🖤</t>
+          <t>oh fuck 🖤</t>
         </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
@@ -814,7 +814,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>look what you made me do 🖤</t>
+          <t>look at what you're doing to me... I can't hold back anymore 💜</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="B17" s="6" t="inlineStr">
         <is>
-          <t>tell me what you'd want me to do to myself right now</t>
+          <t>what would you do if you were here right now babe? I need to hear it</t>
         </is>
       </c>
       <c r="C17" s="6" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>I'm so turned on right now and it's literally your fault</t>
+          <t>I'm dripping wet and every time I think about you watching me it gets worse 💜</t>
         </is>
       </c>
       <c r="C18" s="5" t="inlineStr"/>
@@ -878,7 +878,7 @@
       </c>
       <c r="B19" s="6" t="inlineStr">
         <is>
-          <t>omg okay you're literally making me feel things rn and I can't help it 🖤</t>
+          <t>but I literally can't stop touching myself right now... it's like my body won't let me</t>
         </is>
       </c>
       <c r="C19" s="6" t="inlineStr">
@@ -895,7 +895,7 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>did you see it? 🥺</t>
+          <t>wow... okay I need a second after that 🖤</t>
         </is>
       </c>
       <c r="C20" s="5" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>I literally never show anyone this but you're different</t>
+          <t>I want to show you what you made me feel 💜</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="B23" s="6" t="inlineStr">
         <is>
-          <t>I'm feeling kinda naughty rn... wanna see what I do when I'm bored in bed? 😏</t>
+          <t>I'm lying here and my fingers are starting to wander... I blame you for this babe</t>
         </is>
       </c>
       <c r="C23" s="6" t="inlineStr"/>
@@ -959,7 +959,7 @@
       </c>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>hehe I knew you'd like that 💜</t>
+          <t>my skin is tingling everywhere right now and I can feel my heartbeat getting faster... you're doing something to me</t>
         </is>
       </c>
       <c r="C24" s="5" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="B25" s="6" t="inlineStr">
         <is>
-          <t>sooo?</t>
+          <t>mmm you liked that? that's making me feel way braver than usual 🖤</t>
         </is>
       </c>
       <c r="C25" s="6" t="inlineStr">

</xml_diff>

<commit_message>
fix: round 2 intensity refinement - S1-1/S1-12/S1-15/S1-18 across 21 models (82 fixes)
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/antonella/Antonella_Complete_Infloww.xlsx
+++ b/antonella/Antonella_Complete_Infloww.xlsx
@@ -703,7 +703,7 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>oh my god I can't take it 🖤</t>
+          <t>oh my god I can't stop shaking... I can feel it everywhere 🖤</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>I'm about to lose it... you need to see what's happening to me right now</t>
+          <t>I can feel myself about to cum... you need to see what's happening to my body right now</t>
         </is>
       </c>
       <c r="C11" s="6" t="inlineStr"/>
@@ -797,7 +797,7 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>oh fuck 🖤</t>
+          <t>oh fuck I can't stop touching myself 🖤</t>
         </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="B25" s="6" t="inlineStr">
         <is>
-          <t>mmm you liked that? that's making me feel way braver than usual 🖤</t>
+          <t>mmm you liked that? my body is already reacting to you... I can literally feel myself getting wet right now 🖤</t>
         </is>
       </c>
       <c r="C25" s="6" t="inlineStr">

</xml_diff>

<commit_message>
fix: Phase 4 genuine 10/10 graphic + intensity meter bars in HTML guides
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/antonella/Antonella_Complete_Infloww.xlsx
+++ b/antonella/Antonella_Complete_Infloww.xlsx
@@ -643,7 +643,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>let go with me babe... I need you to see this 💜</t>
+          <t>cum with me babe... watch what happens to my body right now 💜</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -677,7 +677,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>I'm cumming... right now... don't look away</t>
+          <t>I'm cumming... fuck my pussy is pulsing so hard and I can barely breathe</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr"/>
@@ -690,7 +690,7 @@
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>I'm right there babe... don't go anywhere, I need you to watch me finish 💜</t>
+          <t>I'm right there babe... my whole body is clenching around my fingers and I need you watching when I cum 💜</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr"/>
@@ -703,7 +703,7 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>oh my god I can't stop shaking... I can feel it everywhere 🖤</t>
+          <t>oh my god my pussy is pulsing so hard around my fingers and I can't stop 🖤</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">

</xml_diff>

<commit_message>
feat: upgrade OBJ handlers - add descriptions, fix /slash, tone 7/10 challenging
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/antonella/Antonella_Complete_Infloww.xlsx
+++ b/antonella/Antonella_Complete_Infloww.xlsx
@@ -38,10 +38,9 @@
     <sheet name="customno2" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="done1" sheetId="30" state="visible" r:id="rId30"/>
     <sheet name="done2" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="cumcontrol1" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="cumcontrol2" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="dickpic" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="boosters" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="cumcontrol" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="dickpic" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="boosters" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1206,7 +1205,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>it's okay, I'm not going anywhere... let's just keep talking, I like this 💜</t>
+          <t>I'll keep it then, but just know I made it thinking about you</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1224,7 +1223,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>I literally just did this because of what YOU said to me, this wasn't random content babe</t>
+          <t>I literally spent time making this because of what YOU said to me, this wasn't random content, this was for you</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1242,7 +1241,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>free? nah I don't just show this to anyone... you gotta earn the good stuff 😏</t>
+          <t>free? I don't just hand this out, you have to earn the best stuff from me</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1260,12 +1259,12 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>I already sent you one for free remember? this one is way crazier 🖤</t>
+          <t>baby I already gave you one for free remember? this one is on another level and you know it</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>REMINDER. Still wants free → Step 2.</t>
+          <t>REMINDER. Still → Step 2.</t>
         </is>
       </c>
       <c r="D5" s="11" t="inlineStr"/>
@@ -1325,7 +1324,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>no pressure at all, I'm just enjoying talking to you honestly 💜</t>
+          <t>okay I'll hold onto it, but it's got your name on it</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1343,7 +1342,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>I did this because of you... specifically because of our convo, that took effort and I did it for YOU 🥺</t>
+          <t>I recorded this because of our conversation, specifically because of YOU, it took effort and I did it for you</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1361,7 +1360,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>free? you really think the best things in life are free? not this one 🖤</t>
+          <t>the best things aren't free baby, especially not what I just did</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1379,7 +1378,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>you already got a free one, this one is on a whole different level hehe</t>
+          <t>you already got a free preview and this is ten times crazier, you know I don't do free twice</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
@@ -1444,12 +1443,12 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>honestly it's fine, I like talking to you money or not... you do something to me 💜</t>
+          <t>it's fine, you're still here and that's what matters to me right now</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>PROTECT. GFE.</t>
+          <t>PROTECT.</t>
         </is>
       </c>
       <c r="D2" s="11" t="inlineStr"/>
@@ -1462,7 +1461,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>just send whatever you can, even a tiny amount, I just need you to see what you made me do</t>
+          <t>send whatever you can, even something small, I just need you to see what you made me do</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1480,12 +1479,12 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>not even like [small amount]? I really want you to see this one 🥺</t>
+          <t>not even [small amount]? I really want you to be the one who sees this</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>TEST. $3-5. Still no → Step 3.</t>
+          <t>TEST $3-5. Still no → Step 3.</t>
         </is>
       </c>
       <c r="D4" s="11" t="inlineStr"/>
@@ -1498,12 +1497,12 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>hey I totally get it, no pressure at all okay? 🖤</t>
+          <t>I hear you baby, that's okay</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>EMPATHY. Still engaged → Step 2.</t>
+          <t>EMPATHY. Still → Step 2.</t>
         </is>
       </c>
       <c r="D5" s="11" t="inlineStr"/>
@@ -1563,7 +1562,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>it's totally fine, you being here is what matters to me 💜</t>
+          <t>you being here talking to me is enough for now</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1581,7 +1580,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>send whatever feels right, even $1... I just can't keep this from you</t>
+          <t>just send whatever feels right, I can't keep this from you</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1599,7 +1598,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>what about just [small amount]? I really don't want you to miss this 🥺</t>
+          <t>what about just [small amount]? I'd hate for you to miss this one</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1617,7 +1616,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>that's fine babe, seriously don't worry about it 🖤</t>
+          <t>okay don't stress about it</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
@@ -1682,7 +1681,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>just send whatever you want, even $1, I can't keep this to myself... you need to see it</t>
+          <t>send me whatever you want, literally anything, I just can't keep this to myself, you need to see it</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1700,7 +1699,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>look this isn't about money... I just need you to see what you're doing to me right now, I don't react like this to people 🥺</t>
+          <t>okay forget about money, this isn't about that, I need you to see what you're doing to me rn because I've never reacted like this</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1718,7 +1717,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>that's totally fine I'm not trying to sell you anything, I just like talking to you 🖤</t>
+          <t>that's fine, I'm not trying to sell you anything, I'm just enjoying this</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1783,7 +1782,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>send me anything, even the smallest amount, I need you to see what you did to me 🥺</t>
+          <t>send anything, even the smallest amount, you need to see what you did to me</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1801,7 +1800,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>forget about money for a sec... I just want to share this with you, what you're making me feel is real 🖤</t>
+          <t>forget the money part for a sec, I want to share this moment with you because what you're making me feel is real</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1819,7 +1818,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>no worries at all cutie, I don't care about that I'm just enjoying this 💜</t>
+          <t>no worries, I don't care about that rn, this convo is what I care about</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1884,7 +1883,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>figure it out soon babe, I'm in this mood and I don't know how long it's gonna last 💜</t>
+          <t>figure it out soon because this mood I'm in right now isn't gonna last and I want you to have it</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1902,12 +1901,12 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>try a different card? I really don't want you to miss this 🖤</t>
+          <t>maybe try a different card? I really don't want you to miss this</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>ALTERNATIVE. Still fails → Step 3.</t>
+          <t>ALTERNATIVE. Still → Step 3.</t>
         </is>
       </c>
       <c r="D3" s="11" t="inlineStr"/>
@@ -1920,12 +1919,12 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>ugh that sucks, happens sometimes though try again it usually works the second time 🥺</t>
+          <t>ugh that's annoying, try again baby it usually works the second time</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>RETRY. Still fails → Step 2.</t>
+          <t>RETRY. Still → Step 2.</t>
         </is>
       </c>
       <c r="D4" s="11" t="inlineStr"/>
@@ -1985,7 +1984,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>I want you to see this before I change my mind, I don't keep stuff like this around forever 🖤</t>
+          <t>baby fix it quick, I don't keep stuff like this around forever</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -2003,12 +2002,12 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>do you have another card you can try? I really want you to see this 🥺</t>
+          <t>do you have another card? because you really don't want to miss what I made for you</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>ALTERNATIVE. Still fails → Step 3.</t>
+          <t>ALTERNATIVE. Still → Step 3.</t>
         </is>
       </c>
       <c r="D3" s="11" t="inlineStr"/>
@@ -2021,12 +2020,12 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>aw that's annoying, it happens a lot just try one more time</t>
+          <t>that happens sometimes, try one more time for me</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
         <is>
-          <t>RETRY. Still fails → Step 2.</t>
+          <t>RETRY. Still → Step 2.</t>
         </is>
       </c>
       <c r="D4" s="11" t="inlineStr"/>
@@ -2086,7 +2085,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>okay I'll chill... for now, no promises though hehe 💜</t>
+          <t>alright I'll behave, for now... no promises though</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2104,7 +2103,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>I can't help it, there's something about you that's messing with my head right now 🖤</t>
+          <t>okay but I can't help it, there's something about you that keeps messing with my head</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2122,12 +2121,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>so tell me more about you... what do you do when you're not making shy gamer girls lose their minds? 😏</t>
+          <t>so tell me more about you... what do you do when you're not making girls on the internet lose focus?</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>SUBTLE TENSION. → Step 3 later.</t>
+          <t>SUBTLE. → Step 3 later.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -2140,12 +2139,12 @@
       </c>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>haha omg okay I got a little carried away, you're just so easy to talk to 🥺</t>
+          <t>haha okay I got a little carried away, you're too easy to talk to</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
         <is>
-          <t>RESPECT. Still no → Step 2.</t>
+          <t>RESPECT. Still → Step 2.</t>
         </is>
       </c>
       <c r="D5" s="12" t="inlineStr"/>
@@ -2205,7 +2204,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>fine I'll stop but don't blame me if it happens again later 😏</t>
+          <t>fine I'll stop, but don't blame me when it happens again</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2223,7 +2222,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>I'm trying to behave but you're making it really hard, there's something about you 💜</t>
+          <t>I'm trying so hard to behave but you make it impossible</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2241,7 +2240,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>okay new topic but first... what's the craziest thing you've ever done? 😏</t>
+          <t>okay new topic, what's the most adventurous thing you've ever done?</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -2259,12 +2258,12 @@
       </c>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>my bad I got ahead of myself, it's your fault for being so fun to talk to 🖤</t>
+          <t>my bad I got ahead of myself, it's your fault for being this fun to talk to</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
         <is>
-          <t>RESPECT. Still no → Step 2.</t>
+          <t>RESPECT. Still → Step 2.</t>
         </is>
       </c>
       <c r="D5" s="12" t="inlineStr"/>
@@ -2466,7 +2465,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>okay wait no I remember now, so like I was saying...</t>
+          <t>okay wait I remember now, so like I was saying...</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2484,7 +2483,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>but hold on you totally distracted me, I was about to tell you something and now I forgot 🥺</t>
+          <t>but wait you totally distracted me, I was about to say something and now you made me lose my train of thought</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2502,12 +2501,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>haha wait that's actually funny omg</t>
+          <t>haha okay that's actually funny</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>ACKNOWLEDGE. Adapt. → Step 2.</t>
+          <t>ACKNOWLEDGE. Adapt to what he said. → Step 2.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -2567,7 +2566,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>okay focus, where was I... oh yeah 💜</t>
+          <t>OKAY focus, where was I... oh yeah</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2585,7 +2584,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>wait no stop you're distracting me from what I was gonna say</t>
+          <t>wait no stop, you're distracting me from what I was going to tell you</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2603,12 +2602,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>lol okay that's random but I kinda love it 🖤</t>
+          <t>omg okay random but I love it</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>ACKNOWLEDGE. → Step 2.</t>
+          <t>ACKNOWLEDGE. Adapt. → Step 2.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -2668,7 +2667,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>I get it there's a lot of fake stuff on here, but you felt something in this convo right? because I did and that's real 💜</t>
+          <t>I get why you'd think that, there's a lot of fake stuff on here, but what we've been talking about felt real to me... didn't it feel real to you?</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2686,7 +2685,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>ask me anything, literally anything about me or my life. I'm an open book</t>
+          <t>ask me anything, literally anything about my life, I'm an open book, go ahead</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2704,12 +2703,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>lol do I look like a bot to you? beep boop hehe... I'm kidding omg 🖤</t>
+          <t>lol do I sound like a robot to you? beep boop... send $5 for human verification haha I'm kidding</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>HUMOR. Still doubts → Step 2.</t>
+          <t>HUMOR. Still → Step 2.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -2769,7 +2768,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>I know there's tons of bots on here but what we've been talking about felt real to me. didn't it feel real to you? 🥺</t>
+          <t>I know there's a lot of bots out here but what we've been talking about... that felt different, you felt it too right?</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2787,7 +2786,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>test me cutie, ask me something only a real person would know. go ahead 😏</t>
+          <t>test me then, ask me something only a real person would know, go ahead</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2805,7 +2804,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>wait you think I'm not real?? that's actually the funniest thing anyone's said to me today omg 🖤</t>
+          <t>wait you think I'm fake?? that might be the funniest thing anyone's said to me today</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -2870,12 +2869,12 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>I don't do that on here but what I'm about to show you is better than any call babe... you'll see 💜</t>
+          <t>I don't do that on here but what I'm about to show you is better than any call, you'll see</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
         <is>
-          <t>FIRM. Antonella does NOT do video calls.</t>
+          <t>FIRM. No video calls.</t>
         </is>
       </c>
       <c r="D2" s="12" t="inlineStr"/>
@@ -2888,7 +2887,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>I have something way better for you though, trust me you'll forget you even asked 🖤</t>
+          <t>I have something way better for you though, trust me you'll forget you even asked</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2906,12 +2905,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>haha maybe one day if you earn it but not yet... I'm super shy about that stuff 🥺</t>
+          <t>haha maybe one day if you earn it, but not yet</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>DODGE. Still asks → Step 2.</t>
+          <t>DODGE. Model does NOT do video calls. Still → Step 2.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -2971,7 +2970,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>that's not something I do on here but what I have for you is way better than hearing my voice, trust me 💜</t>
+          <t>I don't do that here but trust me what I have is way better than my voice</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2989,7 +2988,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>how about instead of a call I show you something that'll blow your mind? 🖤</t>
+          <t>how about instead of a call I show you something that'll actually blow your mind?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3007,7 +3006,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>hmmm maybe but you gotta earn that first hehe 😏</t>
+          <t>hmmm you gotta earn that first</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3072,7 +3071,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>trust me you won't regret it, I made this one special 💜</t>
+          <t>trust me you won't regret it, I made this one special</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3090,12 +3089,12 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>I have exactly what you're thinking of, you're gonna lose it... [price] 🖤</t>
+          <t>I have it and you're gonna lose your mind... [price]</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>PRICE. Custom min $200. Solo content only.</t>
+          <t>PRICE. Set based on content.</t>
         </is>
       </c>
       <c r="D3" s="12" t="inlineStr"/>
@@ -3108,7 +3107,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>you want that? hmm I might have something... actually I definitely have something 😏</t>
+          <t>mmm you want that? I might have exactly what you're thinking of</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3191,12 +3190,12 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>I actually did something just like that, [price] and it's worth every cent 🖤</t>
+          <t>I made something just like that, [price] and it's worth every penny</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>PRICE. Custom min $200. Solo content only.</t>
+          <t>PRICE.</t>
         </is>
       </c>
       <c r="D3" s="12" t="inlineStr"/>
@@ -3209,7 +3208,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>oh you have good taste... I think I have exactly what you need hehe 💜</t>
+          <t>ohhh you have good taste, I think I know exactly what you need</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3274,7 +3273,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>trust me... I know what you need better than you do 💜</t>
+          <t>trust me, I know what you need better than you do</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3292,7 +3291,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>actually what I have might be even crazier and literally no one else has seen it yet 🖤</t>
+          <t>what I have might be even crazier and literally no one else has seen it</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3310,12 +3309,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>I don't have exactly that but honestly I have something that'll make you forget you even asked 😏</t>
+          <t>I don't have exactly that but I have something that'll make you forget you even asked</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>REDIRECT. Antonella is solo ONLY — redirect any B/G or anal requests here. → Step 2.</t>
+          <t>REDIRECT. → Step 2.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -3375,7 +3374,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>just trust me on this one, you'll thank me later 😏</t>
+          <t>just trust me on this one, you'll thank me after</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3393,7 +3392,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>what I DO have is something no one has ever seen and I think it's even better than what you asked for 💜</t>
+          <t>nobody has seen what I'm about to show you and I think it's better than what you asked for</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3411,12 +3410,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>I don't have that specific thing but I have something you're gonna like even more 🖤</t>
+          <t>hmm not exactly that but what I DO have is gonna hit even harder</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>REDIRECT. Solo only — never acknowledge B/G requests. → Step 2.</t>
+          <t>REDIRECT. → Step 2.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -3688,7 +3687,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>okay but next time you have to wait for me, I have something insane planned for round 2 💜</t>
+          <t>next time you HAVE to wait for me, I have something insane planned for round 2</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3706,12 +3705,12 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>but I haven't finished yet... don't you wanna watch me cum too? 🖤</t>
+          <t>but I haven't finished yet... you're really gonna leave me like this?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
         <is>
-          <t>RESCUE. Solo framing. Still no → Step 3.</t>
+          <t>RESCUE. Still no → Step 3.</t>
         </is>
       </c>
       <c r="D3" s="12" t="inlineStr"/>
@@ -3724,7 +3723,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>wait already?? omg that's so hot 🥺</t>
+          <t>fuck that's so hot, you came because of me??</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3789,7 +3788,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>next time you HAVE to hold it because what I have planned for us is way crazier 💜</t>
+          <t>okay but next time you hold it, because what I have planned is way crazier</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3807,7 +3806,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>wait but I'm not done yet, you're gonna leave me like this? 🖤</t>
+          <t>wait but I'm not done yet, don't you wanna watch me finish too?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3825,7 +3824,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>already?? omg that's hot, because of me?? 🥺</t>
+          <t>already?? damn that's hot</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3890,7 +3889,7 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>if you finish before you see what I'm sending next you'll regret it 💜</t>
+          <t>don't you dare finish before you see this</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
@@ -3908,12 +3907,12 @@
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>wait wait wait... I have one more thing for you before you finish</t>
+          <t>hold it, I want you to wait until you see what I'm about to send, trust me it's worth the wait</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
         <is>
-          <t>DELAY. Send final PPV.</t>
+          <t>DELAY. Send PPV.</t>
         </is>
       </c>
       <c r="D3" s="13" t="inlineStr"/>
@@ -3926,12 +3925,12 @@
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>I want to feel it at the same time... watch this first</t>
+          <t>wait for me, I want us to finish together, open this first</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
         <is>
-          <t>SYNC variant. Send PPV.</t>
+          <t>SYNC variant.</t>
         </is>
       </c>
       <c r="D4" s="13" t="inlineStr"/>
@@ -3944,7 +3943,7 @@
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>okay NOW we can go together... open this 🖤</t>
+          <t>I'm so close too, cum with me... but you need to see this first</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
@@ -3962,7 +3961,7 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>you better not be close already cutie... I have more to show you 💜</t>
+          <t>hold it, not yet... I need you to last longer for me</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
@@ -3980,12 +3979,12 @@
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>not yet... I said not yet 🖤</t>
+          <t>don't cum yet, I'm not done with you</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">
         <is>
-          <t>CONTROL. More PPVs to send. Create urgency to open next.</t>
+          <t>CONTROL.</t>
         </is>
       </c>
       <c r="D7" s="13" t="inlineStr"/>
@@ -4040,17 +4039,17 @@
     <row r="2">
       <c r="A2" s="13" t="inlineStr">
         <is>
-          <t>delay2</t>
+          <t>dpppv2</t>
         </is>
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>hold on just a little longer, I promise this next one is worth it</t>
+          <t>okay you just made me do something, give me a sec</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
         <is>
-          <t>DELAY variant.</t>
+          <t>LEVERAGE variant.</t>
         </is>
       </c>
       <c r="D2" s="13" t="inlineStr"/>
@@ -4058,17 +4057,17 @@
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
         <is>
-          <t>delay1</t>
+          <t>dpppv1</t>
         </is>
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>don't you dare... not until you see what I just did 🖤</t>
+          <t>you can't just send me that and expect me to do nothing about it, hold on...</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
         <is>
-          <t>DELAY. Send PPV.</t>
+          <t>LEVERAGE. WAIT 1-2 min then send PPV.</t>
         </is>
       </c>
       <c r="D3" s="13" t="inlineStr"/>
@@ -4076,17 +4075,17 @@
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
         <is>
-          <t>sync2</t>
+          <t>dprapport2</t>
         </is>
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>let's do this together... but you have to open this first</t>
+          <t>woah I wasn't expecting that but... damn okay</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
         <is>
-          <t>SYNC variant.</t>
+          <t>DURING RAPPORT variant.</t>
         </is>
       </c>
       <c r="D4" s="13" t="inlineStr"/>
@@ -4094,17 +4093,17 @@
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
         <is>
-          <t>sync1</t>
+          <t>dprapport1</t>
         </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>okay I'm ready now too... watch this with me 💜</t>
+          <t>omg you don't waste time huh, that's actually really hot ngl</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
         <is>
-          <t>SYNC. Send PPV.</t>
+          <t>DURING RAPPORT.</t>
         </is>
       </c>
       <c r="D5" s="13" t="inlineStr"/>
@@ -4112,17 +4111,17 @@
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
         <is>
-          <t>edge2</t>
+          <t>dpsext2</t>
         </is>
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>patience... the best part hasn't even happened yet</t>
+          <t>oh fuck that is... damn, I need to show you something rn</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
         <is>
-          <t>EDGE variant.</t>
+          <t>DURING SEXTING variant.</t>
         </is>
       </c>
       <c r="D6" s="13" t="inlineStr"/>
@@ -4130,17 +4129,17 @@
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
         <is>
-          <t>edge1</t>
+          <t>dpsext1</t>
         </is>
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>slow down cutie... I'm not letting you off that easy 🖤</t>
+          <t>fuck okay that's... wow, you have no idea what that just did to me</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">
         <is>
-          <t>CONTROL.</t>
+          <t>DURING SEXTING.</t>
         </is>
       </c>
       <c r="D7" s="13" t="inlineStr"/>
@@ -4151,161 +4150,6 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="80" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="10" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="10" t="inlineStr">
-        <is>
-          <t>Text</t>
-        </is>
-      </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>Note</t>
-        </is>
-      </c>
-      <c r="D1" s="10" t="inlineStr">
-        <is>
-          <t>*Guidelines</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="13" t="inlineStr">
-        <is>
-          <t>dpppv2</t>
-        </is>
-      </c>
-      <c r="B2" s="13" t="inlineStr">
-        <is>
-          <t>okay you just made me do something... give me a sec 🖤</t>
-        </is>
-      </c>
-      <c r="C2" s="13" t="inlineStr">
-        <is>
-          <t>LEVERAGE variant.</t>
-        </is>
-      </c>
-      <c r="D2" s="13" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="13" t="inlineStr">
-        <is>
-          <t>dpppv1</t>
-        </is>
-      </c>
-      <c r="B3" s="13" t="inlineStr">
-        <is>
-          <t>you can't just send me that and expect me not to do something about it, hold on 💜</t>
-        </is>
-      </c>
-      <c r="C3" s="13" t="inlineStr">
-        <is>
-          <t>LEVERAGE. WAIT 1-2 min then send PPV.</t>
-        </is>
-      </c>
-      <c r="D3" s="13" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="13" t="inlineStr">
-        <is>
-          <t>dprapport2</t>
-        </is>
-      </c>
-      <c r="B4" s="13" t="inlineStr">
-        <is>
-          <t>omg I was not expecting that but... damn 🖤</t>
-        </is>
-      </c>
-      <c r="C4" s="13" t="inlineStr">
-        <is>
-          <t>DURING RAPPORT variant.</t>
-        </is>
-      </c>
-      <c r="D4" s="13" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="inlineStr">
-        <is>
-          <t>dprapport1</t>
-        </is>
-      </c>
-      <c r="B5" s="13" t="inlineStr">
-        <is>
-          <t>woah you don't waste time huh? that's actually really hot though ngl 🥺</t>
-        </is>
-      </c>
-      <c r="C5" s="13" t="inlineStr">
-        <is>
-          <t>DURING RAPPORT. She's 'shy' but reacts positively.</t>
-        </is>
-      </c>
-      <c r="D5" s="13" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="13" t="inlineStr">
-        <is>
-          <t>dpsext2</t>
-        </is>
-      </c>
-      <c r="B6" s="13" t="inlineStr">
-        <is>
-          <t>oh my god... that is... damn. I need to show you something right now 💜</t>
-        </is>
-      </c>
-      <c r="C6" s="13" t="inlineStr">
-        <is>
-          <t>DURING SEXTING variant.</t>
-        </is>
-      </c>
-      <c r="D6" s="13" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="13" t="inlineStr">
-        <is>
-          <t>dpsext1</t>
-        </is>
-      </c>
-      <c r="B7" s="13" t="inlineStr">
-        <is>
-          <t>fuck okay that's... wow. you have no idea what that just did to me 🖤</t>
-        </is>
-      </c>
-      <c r="C7" s="13" t="inlineStr">
-        <is>
-          <t>DURING SEXTING. React positively, leverage into PPV.</t>
-        </is>
-      </c>
-      <c r="D7" s="13" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4355,12 +4199,12 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>I should be gaming rn but I can't even hold my controller 🖤</t>
+          <t>I literally can't focus on anything else rn</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
         <is>
-          <t>BOOSTER. Antonella personality — gaming reference.</t>
+          <t>BOOSTER.</t>
         </is>
       </c>
       <c r="D2" s="13" t="inlineStr"/>
@@ -4373,7 +4217,7 @@
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>again...</t>
+          <t>more</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
@@ -4391,7 +4235,7 @@
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>my legs are shaking</t>
+          <t>my hands are shaking</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
@@ -4409,7 +4253,7 @@
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>I literally can't think straight right now 💜</t>
+          <t>I can't think straight rn</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
@@ -4427,7 +4271,7 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>I literally can't handle this right now</t>
+          <t>you have no idea what you're doing to me</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
@@ -4445,7 +4289,7 @@
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>keep going</t>
+          <t>don't stop</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">
@@ -4463,7 +4307,7 @@
       </c>
       <c r="B8" s="13" t="inlineStr">
         <is>
-          <t>I'm so wet right now because of you</t>
+          <t>I'm so wet rn because of you</t>
         </is>
       </c>
       <c r="C8" s="13" t="inlineStr">
@@ -4481,7 +4325,7 @@
       </c>
       <c r="B9" s="13" t="inlineStr">
         <is>
-          <t>fuckkk 🖤</t>
+          <t>fuckkk</t>
         </is>
       </c>
       <c r="C9" s="13" t="inlineStr">
@@ -4832,7 +4676,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>it's okay love, let's just keep talking... I'm still thinking about you anyway 💜</t>
+          <t>alright, I'll keep it then... but next time I'm in this mood you better be ready</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -4850,7 +4694,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>okay fine [lower price] just for you because this convo has been different 🖤</t>
+          <t>fine, [lower price] but only because you've been making me feel some type of way, don't tell anyone I did this</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -4868,7 +4712,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>maybe you're just not ready for what I did in this one 😏</t>
+          <t>honestly? most guys couldn't handle what I just recorded... I thought you were different</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -4886,7 +4730,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>I'm only in this mood because of you rn, I don't know when this is gonna happen again 🥺</t>
+          <t>I'm literally dripping rn because of what you said and this mood isn't gonna last, don't miss it</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
@@ -4904,12 +4748,12 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>babe that's less than like a boba and trust me this hits way harder hehe</t>
+          <t>babe that's less than your morning coffee and I promise this is gonna keep you up way longer</t>
         </is>
       </c>
       <c r="C6" s="11" t="inlineStr">
         <is>
-          <t>REFRAME. Wait. Still no → Step 2.</t>
+          <t>REFRAME. Still no → Step 2.</t>
         </is>
       </c>
       <c r="D6" s="11" t="inlineStr"/>
@@ -4969,7 +4813,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>no pressure cutie, I like talking to you regardless 💜</t>
+          <t>I'll hold onto it for now, but I know you're gonna come back for it</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -4987,7 +4831,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>okay fine [lower price] because you've been making me feel some type of way, but keep that between us 🥺</t>
+          <t>look, [lower price] because I actually want YOU to have this one, I'm not doing this for anyone else</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -5005,7 +4849,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>most guys can't handle what I just did, I thought you were different</t>
+          <t>maybe you're just not ready for what I did... it's a lot</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -5023,7 +4867,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>this mood won't last forever and I want you to be the one who sees it 🖤</t>
+          <t>this mood won't last and I already picked YOU to share it with, don't make me regret that</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
@@ -5041,7 +4885,7 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>that's literally what you'd spend on a snack and this is gonna keep you up all night</t>
+          <t>baby it's literally nothing for what you're about to see, trust me you'll be thanking me after</t>
         </is>
       </c>
       <c r="C6" s="11" t="inlineStr">
@@ -5106,12 +4950,12 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>if you don't want it that's okay, I'll keep it for myself... or maybe someone else who's been asking 💜</t>
+          <t>okay I'll just save this for someone who actually wants it then, their loss isn't your gain though</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
         <is>
-          <t>TAKEAWAY. Final.</t>
+          <t>TAKEAWAY.</t>
         </is>
       </c>
       <c r="D2" s="11" t="inlineStr"/>
@@ -5124,7 +4968,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>fine [lower price] just for you but shhh this stays between us okay? 🥺</t>
+          <t>ugh fine, [lower price] ONLY because I like you but don't ever ask me this again</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -5142,7 +4986,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>I don't do discounts... I only share this with guys who actually appreciate what they're getting 🖤</t>
+          <t>the guys who get my best stuff don't ask for discounts, they know what they're getting</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -5160,12 +5004,12 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>haha are you trying to haggle with me?? this isn't a game babe, it's worth every cent 😏</t>
+          <t>haha negotiate? baby this isn't a flea market... you already know this is worth every penny</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>FIRMNESS. Still pushing → Step 2.</t>
+          <t>FIRMNESS. Still → Step 2.</t>
         </is>
       </c>
       <c r="D5" s="11" t="inlineStr"/>
@@ -5225,7 +5069,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>alright I'll save it for someone who actually wants it then</t>
+          <t>no worries, I'll keep it... someone else has been asking and they won't hesitate</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -5243,7 +5087,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>okay [lower price] but ONLY because I like you, one time thing 🥺</t>
+          <t>okay [lower price] and that's ONLY because this convo has been different, first and last time</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -5261,7 +5105,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>the guys who appreciate what I do never ask for discounts, just saying 🖤</t>
+          <t>I don't do this for just anyone, and the ones who get it never complain about the price after</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -5279,7 +5123,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>a discount? do I look like I'm on sale cutie? 😏</t>
+          <t>a discount? babe do I look like I'm on sale? you know exactly what you're getting</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">

</xml_diff>

<commit_message>
fix: unique command names in XLSX - prefix protocol name to each step
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/antonella/Antonella_Complete_Infloww.xlsx
+++ b/antonella/Antonella_Complete_Infloww.xlsx
@@ -1200,7 +1200,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Seed</t>
+          <t>free1 Step4 Seed</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -1218,7 +1218,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 Guilt</t>
+          <t>free1 Step3 Guilt</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -1236,7 +1236,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>free1 Step2 Challenge</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -1254,7 +1254,7 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Reminder</t>
+          <t>free1 Step1 Reminder</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
@@ -1319,7 +1319,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Seed</t>
+          <t>free2 Step4 Seed</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -1337,7 +1337,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 Guilt</t>
+          <t>free2 Step3 Guilt</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -1355,7 +1355,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>free2 Step2 Challenge</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -1373,7 +1373,7 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Reminder</t>
+          <t>free2 Step1 Reminder</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
@@ -1438,7 +1438,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Protect</t>
+          <t>nomoney1 Step4 Protect</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -1456,7 +1456,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 PWYW</t>
+          <t>nomoney1 Step3 PWYW</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -1474,7 +1474,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Test</t>
+          <t>nomoney1 Step2 Test</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Empathy</t>
+          <t>nomoney1 Step1 Empathy</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
@@ -1557,7 +1557,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Protect</t>
+          <t>nomoney2 Step4 Protect</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -1575,7 +1575,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 PWYW</t>
+          <t>nomoney2 Step3 PWYW</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -1593,7 +1593,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Test</t>
+          <t>nomoney2 Step2 Test</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -1611,7 +1611,7 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Empathy</t>
+          <t>nomoney2 Step1 Empathy</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
@@ -1676,7 +1676,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step3 PWYW</t>
+          <t>noppv1 Step3 PWYW</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -1694,7 +1694,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step2 Reframe</t>
+          <t>noppv1 Step2 Reframe</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -1712,7 +1712,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step1 Accept</t>
+          <t>noppv1 Step1 Accept</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -1777,7 +1777,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step3 PWYW</t>
+          <t>noppv2 Step3 PWYW</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -1795,7 +1795,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step2 Reframe</t>
+          <t>noppv2 Step2 Reframe</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -1813,7 +1813,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step1 Accept</t>
+          <t>noppv2 Step1 Accept</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -1878,7 +1878,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step3 Urgency</t>
+          <t>card1 Step3 Urgency</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -1896,7 +1896,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step2 AltCard</t>
+          <t>card1 Step2 AltCard</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -1914,7 +1914,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step1 Retry</t>
+          <t>card1 Step1 Retry</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -1979,7 +1979,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step3 Urgency</t>
+          <t>card2 Step3 Urgency</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -1997,7 +1997,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step2 AltCard</t>
+          <t>card2 Step2 AltCard</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -2015,7 +2015,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step1 Retry</t>
+          <t>card2 Step1 Retry</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -2080,7 +2080,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step4 Accept</t>
+          <t>nosex1 Step4 Accept</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -2098,7 +2098,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step3 ReAttempt</t>
+          <t>nosex1 Step3 ReAttempt</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -2116,7 +2116,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step2 Subtle</t>
+          <t>nosex1 Step2 Subtle</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -2134,7 +2134,7 @@
     <row r="5">
       <c r="A5" s="12" t="inlineStr">
         <is>
-          <t>Step1 Respect</t>
+          <t>nosex1 Step1 Respect</t>
         </is>
       </c>
       <c r="B5" s="12" t="inlineStr">
@@ -2199,7 +2199,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step4 Accept</t>
+          <t>nosex2 Step4 Accept</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -2217,7 +2217,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step3 ReAttempt</t>
+          <t>nosex2 Step3 ReAttempt</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -2235,7 +2235,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step2 Subtle</t>
+          <t>nosex2 Step2 Subtle</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -2253,7 +2253,7 @@
     <row r="5">
       <c r="A5" s="12" t="inlineStr">
         <is>
-          <t>Step1 Respect</t>
+          <t>nosex2 Step1 Respect</t>
         </is>
       </c>
       <c r="B5" s="12" t="inlineStr">
@@ -2460,7 +2460,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Retake</t>
+          <t>offtopic1 Step3 Retake</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -2478,7 +2478,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Redirect</t>
+          <t>offtopic1 Step2 Redirect</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -2496,7 +2496,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Acknowledge</t>
+          <t>offtopic1 Step1 Acknowledge</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -2561,7 +2561,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Retake</t>
+          <t>offtopic2 Step3 Retake</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -2579,7 +2579,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Redirect</t>
+          <t>offtopic2 Step2 Redirect</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -2597,7 +2597,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Acknowledge</t>
+          <t>offtopic2 Step1 Acknowledge</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -2662,7 +2662,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Grounding</t>
+          <t>real1 Step3 Grounding</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -2680,7 +2680,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>real1 Step2 Challenge</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -2698,7 +2698,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Humor</t>
+          <t>real1 Step1 Humor</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -2763,7 +2763,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Grounding</t>
+          <t>real2 Step3 Grounding</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -2781,7 +2781,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>real2 Step2 Challenge</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -2799,7 +2799,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Humor</t>
+          <t>real2 Step1 Humor</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -2864,7 +2864,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Firm</t>
+          <t>voice1 Step3 Firm</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -2882,7 +2882,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Redirect</t>
+          <t>voice1 Step2 Redirect</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -2900,7 +2900,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Dodge</t>
+          <t>voice1 Step1 Dodge</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -2965,7 +2965,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Firm</t>
+          <t>voice2 Step3 Firm</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -2983,7 +2983,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Redirect</t>
+          <t>voice2 Step2 Redirect</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -3001,7 +3001,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Dodge</t>
+          <t>voice2 Step1 Dodge</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -3066,7 +3066,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Close</t>
+          <t>customyes1 Step3 Close</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -3084,7 +3084,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Price</t>
+          <t>customyes1 Step2 Price</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -3102,7 +3102,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Tease</t>
+          <t>customyes1 Step1 Tease</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -3167,7 +3167,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Close</t>
+          <t>customyes2 Step3 Close</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -3185,7 +3185,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Price</t>
+          <t>customyes2 Step2 Price</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -3203,7 +3203,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Tease</t>
+          <t>customyes2 Step1 Tease</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -3268,7 +3268,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Close</t>
+          <t>customno1 Step3 Close</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -3286,7 +3286,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Alternative</t>
+          <t>customno1 Step2 Alternative</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -3304,7 +3304,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Redirect</t>
+          <t>customno1 Step1 Redirect</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -3369,7 +3369,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Close</t>
+          <t>customno2 Step3 Close</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -3387,7 +3387,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Alternative</t>
+          <t>customno2 Step2 Alternative</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -3405,7 +3405,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Redirect</t>
+          <t>customno2 Step1 Redirect</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -3682,7 +3682,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Seed</t>
+          <t>done1 Step3 Seed</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -3700,7 +3700,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Rescue</t>
+          <t>done1 Step2 Rescue</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -3718,7 +3718,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Validate</t>
+          <t>done1 Step1 Validate</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -3783,7 +3783,7 @@
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
         <is>
-          <t>Step3 Seed</t>
+          <t>done2 Step3 Seed</t>
         </is>
       </c>
       <c r="B2" s="12" t="inlineStr">
@@ -3801,7 +3801,7 @@
     <row r="3">
       <c r="A3" s="12" t="inlineStr">
         <is>
-          <t>Step2 Rescue</t>
+          <t>done2 Step2 Rescue</t>
         </is>
       </c>
       <c r="B3" s="12" t="inlineStr">
@@ -3819,7 +3819,7 @@
     <row r="4">
       <c r="A4" s="12" t="inlineStr">
         <is>
-          <t>Step1 Validate</t>
+          <t>done2 Step1 Validate</t>
         </is>
       </c>
       <c r="B4" s="12" t="inlineStr">
@@ -3884,7 +3884,7 @@
     <row r="2">
       <c r="A2" s="13" t="inlineStr">
         <is>
-          <t>delay2</t>
+          <t>cumcontrol delay2</t>
         </is>
       </c>
       <c r="B2" s="13" t="inlineStr">
@@ -3902,7 +3902,7 @@
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
         <is>
-          <t>delay1</t>
+          <t>cumcontrol delay1</t>
         </is>
       </c>
       <c r="B3" s="13" t="inlineStr">
@@ -3920,7 +3920,7 @@
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
         <is>
-          <t>sync2</t>
+          <t>cumcontrol sync2</t>
         </is>
       </c>
       <c r="B4" s="13" t="inlineStr">
@@ -3938,7 +3938,7 @@
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
         <is>
-          <t>sync1</t>
+          <t>cumcontrol sync1</t>
         </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
@@ -3956,7 +3956,7 @@
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
         <is>
-          <t>edge2</t>
+          <t>cumcontrol edge2</t>
         </is>
       </c>
       <c r="B6" s="13" t="inlineStr">
@@ -3974,7 +3974,7 @@
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
         <is>
-          <t>edge1</t>
+          <t>cumcontrol edge1</t>
         </is>
       </c>
       <c r="B7" s="13" t="inlineStr">
@@ -4039,7 +4039,7 @@
     <row r="2">
       <c r="A2" s="13" t="inlineStr">
         <is>
-          <t>dpppv2</t>
+          <t>dickpic dpppv2</t>
         </is>
       </c>
       <c r="B2" s="13" t="inlineStr">
@@ -4057,7 +4057,7 @@
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
         <is>
-          <t>dpppv1</t>
+          <t>dickpic dpppv1</t>
         </is>
       </c>
       <c r="B3" s="13" t="inlineStr">
@@ -4075,7 +4075,7 @@
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
         <is>
-          <t>dprapport2</t>
+          <t>dickpic dprapport2</t>
         </is>
       </c>
       <c r="B4" s="13" t="inlineStr">
@@ -4093,7 +4093,7 @@
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
         <is>
-          <t>dprapport1</t>
+          <t>dickpic dprapport1</t>
         </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
@@ -4111,7 +4111,7 @@
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
         <is>
-          <t>dpsext2</t>
+          <t>dickpic dpsext2</t>
         </is>
       </c>
       <c r="B6" s="13" t="inlineStr">
@@ -4129,7 +4129,7 @@
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
         <is>
-          <t>dpsext1</t>
+          <t>dickpic dpsext1</t>
         </is>
       </c>
       <c r="B7" s="13" t="inlineStr">
@@ -4194,7 +4194,7 @@
     <row r="2">
       <c r="A2" s="13" t="inlineStr">
         <is>
-          <t>h8</t>
+          <t>boosters h8</t>
         </is>
       </c>
       <c r="B2" s="13" t="inlineStr">
@@ -4212,7 +4212,7 @@
     <row r="3">
       <c r="A3" s="13" t="inlineStr">
         <is>
-          <t>h7</t>
+          <t>boosters h7</t>
         </is>
       </c>
       <c r="B3" s="13" t="inlineStr">
@@ -4230,7 +4230,7 @@
     <row r="4">
       <c r="A4" s="13" t="inlineStr">
         <is>
-          <t>h6</t>
+          <t>boosters h6</t>
         </is>
       </c>
       <c r="B4" s="13" t="inlineStr">
@@ -4248,7 +4248,7 @@
     <row r="5">
       <c r="A5" s="13" t="inlineStr">
         <is>
-          <t>h5</t>
+          <t>boosters h5</t>
         </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
@@ -4266,7 +4266,7 @@
     <row r="6">
       <c r="A6" s="13" t="inlineStr">
         <is>
-          <t>h4</t>
+          <t>boosters h4</t>
         </is>
       </c>
       <c r="B6" s="13" t="inlineStr">
@@ -4284,7 +4284,7 @@
     <row r="7">
       <c r="A7" s="13" t="inlineStr">
         <is>
-          <t>h3</t>
+          <t>boosters h3</t>
         </is>
       </c>
       <c r="B7" s="13" t="inlineStr">
@@ -4302,7 +4302,7 @@
     <row r="8">
       <c r="A8" s="13" t="inlineStr">
         <is>
-          <t>h2</t>
+          <t>boosters h2</t>
         </is>
       </c>
       <c r="B8" s="13" t="inlineStr">
@@ -4320,7 +4320,7 @@
     <row r="9">
       <c r="A9" s="13" t="inlineStr">
         <is>
-          <t>h1</t>
+          <t>boosters h1</t>
         </is>
       </c>
       <c r="B9" s="13" t="inlineStr">
@@ -4671,7 +4671,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step5 Seed</t>
+          <t>price1 Step5 Seed</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -4689,7 +4689,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step4 Downgrade</t>
+          <t>price1 Step4 Downgrade</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -4707,7 +4707,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step3 Challenge</t>
+          <t>price1 Step3 Challenge</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -4725,7 +4725,7 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step2 FOMO</t>
+          <t>price1 Step2 FOMO</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
@@ -4743,7 +4743,7 @@
     <row r="6">
       <c r="A6" s="11" t="inlineStr">
         <is>
-          <t>Step1 Reframe</t>
+          <t>price1 Step1 Reframe</t>
         </is>
       </c>
       <c r="B6" s="11" t="inlineStr">
@@ -4808,7 +4808,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step5 Seed</t>
+          <t>price2 Step5 Seed</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -4826,7 +4826,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step4 Downgrade</t>
+          <t>price2 Step4 Downgrade</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -4844,7 +4844,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step3 Challenge</t>
+          <t>price2 Step3 Challenge</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -4862,7 +4862,7 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step2 FOMO</t>
+          <t>price2 Step2 FOMO</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
@@ -4880,7 +4880,7 @@
     <row r="6">
       <c r="A6" s="11" t="inlineStr">
         <is>
-          <t>Step1 Reframe</t>
+          <t>price2 Step1 Reframe</t>
         </is>
       </c>
       <c r="B6" s="11" t="inlineStr">
@@ -4945,7 +4945,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Takeaway</t>
+          <t>discount1 Step4 Takeaway</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -4963,7 +4963,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 Concession</t>
+          <t>discount1 Step3 Concession</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -4981,7 +4981,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>discount1 Step2 Challenge</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -4999,7 +4999,7 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Firmness</t>
+          <t>discount1 Step1 Firmness</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">
@@ -5064,7 +5064,7 @@
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
         <is>
-          <t>Step4 Takeaway</t>
+          <t>discount2 Step4 Takeaway</t>
         </is>
       </c>
       <c r="B2" s="11" t="inlineStr">
@@ -5082,7 +5082,7 @@
     <row r="3">
       <c r="A3" s="11" t="inlineStr">
         <is>
-          <t>Step3 Concession</t>
+          <t>discount2 Step3 Concession</t>
         </is>
       </c>
       <c r="B3" s="11" t="inlineStr">
@@ -5100,7 +5100,7 @@
     <row r="4">
       <c r="A4" s="11" t="inlineStr">
         <is>
-          <t>Step2 Challenge</t>
+          <t>discount2 Step2 Challenge</t>
         </is>
       </c>
       <c r="B4" s="11" t="inlineStr">
@@ -5118,7 +5118,7 @@
     <row r="5">
       <c r="A5" s="11" t="inlineStr">
         <is>
-          <t>Step1 Firmness</t>
+          <t>discount2 Step1 Firmness</t>
         </is>
       </c>
       <c r="B5" s="11" t="inlineStr">

</xml_diff>